<commit_message>
added stimuli to training session
</commit_message>
<xml_diff>
--- a/01_Paradigms/ER-ED/ER_Training/Stimuli_distance.xlsx
+++ b/01_Paradigms/ER-ED/ER_Training/Stimuli_distance.xlsx
@@ -5,7 +5,7 @@
   <workbookPr defaultThemeVersion="164011"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\scheffel\Scheffel\Forschung\A_Projects\2021_COG-ER-ED\COG-ER-ED\01_Paradigms\ER-ED\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\scheffel\Scheffel\Forschung\A_Projects\2021_COG-ER-ED\COG-ER-ED\01_Paradigms\ER-ED\ER_Training\"/>
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
@@ -15,7 +15,7 @@
     <sheet name="Tabelle1" sheetId="1" r:id="rId1"/>
     <sheet name="Tabelle2" sheetId="2" r:id="rId2"/>
   </sheets>
-  <calcPr calcId="162913" iterateDelta="1E-4"/>
+  <calcPr calcId="162913"/>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="207" uniqueCount="9">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="208" uniqueCount="10">
   <si>
     <t>ImageFile</t>
   </si>
@@ -42,16 +42,19 @@
     <t>.jpg</t>
   </si>
   <si>
-    <t>Stimuli/242.jpg</t>
+    <t>Stimuli/224.jpg</t>
   </si>
   <si>
-    <t>Stimuli/252.jpg</t>
+    <t>Stimuli/1271.jpg</t>
   </si>
   <si>
-    <t>Stimuli/3001.jpg</t>
+    <t>Stimuli/2301.jpg</t>
   </si>
   <si>
-    <t>StimSet</t>
+    <t>Stimuli/2688.jpg</t>
+  </si>
+  <si>
+    <t>Stimuli/8485.jpg</t>
   </si>
 </sst>
 </file>
@@ -371,44 +374,45 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:B4"/>
+  <dimension ref="A1:B6"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="E8" sqref="E8"/>
+      <selection activeCell="A7" sqref="A7"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <sheetData>
     <row r="1" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A1" t="s">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="2" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A2" s="1" t="s">
+        <v>5</v>
+      </c>
+      <c r="B2" s="1"/>
+    </row>
+    <row r="3" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A3" s="1" t="s">
+        <v>6</v>
+      </c>
+      <c r="B3" s="1"/>
+    </row>
+    <row r="4" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A4" s="1" t="s">
+        <v>7</v>
+      </c>
+      <c r="B4" s="1"/>
+    </row>
+    <row r="5" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A5" s="1" t="s">
         <v>8</v>
       </c>
-      <c r="B1" t="s">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="2" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A2">
-        <v>3</v>
-      </c>
-      <c r="B2" t="s">
-        <v>5</v>
-      </c>
-    </row>
-    <row r="3" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A3">
-        <v>3</v>
-      </c>
-      <c r="B3" t="s">
-        <v>6</v>
-      </c>
-    </row>
-    <row r="4" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A4">
-        <v>3</v>
-      </c>
-      <c r="B4" t="s">
-        <v>7</v>
+    </row>
+    <row r="6" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A6" s="1" t="s">
+        <v>9</v>
       </c>
     </row>
   </sheetData>

</xml_diff>